<commit_message>
Update with complete forumla. Makes it a bit more plug and play
</commit_message>
<xml_diff>
--- a/IEEE-754/IEEE-754.xlsx
+++ b/IEEE-754/IEEE-754.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Google Drive/School/CS190/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Workspace/cs190/IEEE-754/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="8880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="8880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Decimal -&gt; IEEE-754" sheetId="1" r:id="rId1"/>
@@ -139,11 +139,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="A1:AJ3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,41 +443,41 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
       <c r="AG1" s="1" t="s">
         <v>2</v>
       </c>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="AI6" sqref="AI6"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="AI3" sqref="AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,41 +748,41 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
       <c r="AG1" s="4" t="s">
         <v>7</v>
       </c>
@@ -893,14 +893,14 @@
       <c r="AF2">
         <v>0</v>
       </c>
-      <c r="AG2" s="7">
+      <c r="AG2" s="6">
         <v>0</v>
       </c>
       <c r="AH2" s="5">
         <v>130</v>
       </c>
       <c r="AI2" s="5">
-        <f>(J2*2^-1)+(K2*2^-2)+(L2*2^-3)+(M2*2^-4)+(N2*2^-5)+(O2*2^-6)</f>
+        <f>(J2*2^-1)+(K2*2^-2)+(L2*2^-3)+(M2*2^-4)+(N2*2^-5)+(O2*2^-6)+(P2*2^-6)+(Q2*2^-6)+(R2*2^-6)+(S2*2^-6)+(T2*2^-6)+(U2*2^-6)+(V2*2^-6)+(W2*2^-6)+(X2*2^-6)+(Y2*2^-6)+(Z2*2^-6)+(AA2*2^-6)+(AB2*2^-6)+(AC2*2^-6)+(AD2*2^-6)+(AE2*2^-6)+(AF2*2^-6)</f>
         <v>0.234375</v>
       </c>
       <c r="AJ2">
@@ -1005,14 +1005,14 @@
       <c r="AF3">
         <v>0</v>
       </c>
-      <c r="AG3" s="7">
+      <c r="AG3" s="6">
         <v>1</v>
       </c>
       <c r="AH3" s="5">
         <v>131</v>
       </c>
       <c r="AI3" s="5">
-        <f>(J3*2^-1)+(K3*2^-2)+(L3*2^-3)+(M3*2^-4)+(N3*2^-5)+(O3*2^-6)</f>
+        <f>(J3*2^-1)+(K3*2^-2)+(L3*2^-3)+(M3*2^-4)+(N3*2^-5)+(O3*2^-6)+(P3*2^-6)+(Q3*2^-6)+(R3*2^-6)+(S3*2^-6)+(T3*2^-6)+(U3*2^-6)+(V3*2^-6)+(W3*2^-6)+(X3*2^-6)+(Y3*2^-6)+(Z3*2^-6)+(AA3*2^-6)+(AB3*2^-6)+(AC3*2^-6)+(AD3*2^-6)+(AE3*2^-6)+(AF3*2^-6)</f>
         <v>0.703125</v>
       </c>
       <c r="AJ3">

</xml_diff>